<commit_message>
First try to fill excel values
</commit_message>
<xml_diff>
--- a/HW5/instructions/ROC First Step.xlsx
+++ b/HW5/instructions/ROC First Step.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben galili\Dropbox\IDC ML Undergrad\שיעורי בית\HW5\HW5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\arik\git\machineLearningHW\HW5\instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>TPR</t>
   </si>
@@ -50,19 +50,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -122,8 +122,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="טוב" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -144,9 +144,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="he-IL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -188,7 +188,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -214,7 +213,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="he-IL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -266,6 +265,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.17599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -275,10 +292,33 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.47799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.47799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.47799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.34799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F9AF-4635-9CC8-26BCEFB34C79}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -340,7 +380,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -366,7 +405,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="he-IL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -404,7 +443,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="he-IL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="461477072"/>
@@ -461,7 +500,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -487,7 +525,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="he-IL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -525,7 +563,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="he-IL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="461465104"/>
@@ -567,7 +605,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="he-IL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -579,9 +617,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="he-IL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -619,7 +657,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -645,7 +682,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="he-IL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -712,6 +749,60 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.8999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.11799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.11799999999999999</c:v>
+                </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
@@ -724,6 +815,60 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.30399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.34799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.435</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.52200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.47799999999999998</c:v>
+                </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
@@ -731,6 +876,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B23F-49D5-BA6C-0CE727ECDCA0}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -792,7 +942,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -818,7 +967,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="he-IL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -856,7 +1005,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="he-IL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="461462928"/>
@@ -914,7 +1063,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -940,7 +1088,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="he-IL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -978,7 +1126,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="he-IL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="461463472"/>
@@ -1020,7 +1168,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="he-IL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2160,20 +2308,32 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="קבוצה 1"/>
+        <xdr:cNvPr id="2" name="קבוצה 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4922520" y="365760"/>
-          <a:ext cx="4572000" cy="4065270"/>
+          <a:off x="4495800" y="396240"/>
+          <a:ext cx="4145280" cy="4415790"/>
           <a:chOff x="5707380" y="365760"/>
           <a:chExt cx="4572000" cy="4065270"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:graphicFrame macro="">
         <xdr:nvGraphicFramePr>
-          <xdr:cNvPr id="3" name="תרשים 2"/>
+          <xdr:cNvPr id="3" name="תרשים 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvGraphicFramePr/>
         </xdr:nvGraphicFramePr>
         <xdr:xfrm>
@@ -2188,7 +2348,13 @@
       </xdr:graphicFrame>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="5" name="מחבר ישר 4"/>
+          <xdr:cNvPr id="5" name="מחבר ישר 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -2233,7 +2399,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="18" name="תרשים 17"/>
+        <xdr:cNvPr id="18" name="תרשים 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2246,6 +2418,56 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>450895</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85042</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="מחבר ישר 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57C2C5CF-77E0-447E-A4D8-ADB338BDEE87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5105400" y="904875"/>
+          <a:ext cx="2317795" cy="2228167"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2516,13 +2738,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
@@ -2544,8 +2766,12 @@
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="2">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.17599999999999999</v>
+      </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -2554,8 +2780,12 @@
       <c r="D6">
         <v>3</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="2">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.17599999999999999</v>
+      </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -2564,8 +2794,12 @@
       <c r="D7">
         <v>4</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="2">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.17599999999999999</v>
+      </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
@@ -2574,8 +2808,12 @@
       <c r="D8">
         <v>0.01</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
@@ -2584,8 +2822,12 @@
       <c r="D9">
         <v>0.1</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="2">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2.9000000000000001E-2</v>
+      </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
@@ -2594,8 +2836,12 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
@@ -2612,132 +2858,206 @@
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D17">
         <v>3.3000000000000003E-5</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="E17" s="4">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>6.6000000000000005E-5</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>1E-4</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>3.3E-4</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>6.6E-4</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>1E-3</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>3.3E-3</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D24">
         <v>6.6E-3</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="E24" s="4">
+        <v>1</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D25">
         <v>0.01</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="E26" s="4">
+        <v>1</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="E27" s="4">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>0.1</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="E28" s="4">
+        <v>1</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>0.33</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="E29" s="4">
+        <v>1</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>0.66</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="E30" s="4">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="F30" s="4">
+        <v>2.9000000000000001E-2</v>
+      </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="E31" s="4">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="F31" s="4">
+        <v>2.9000000000000001E-2</v>
+      </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D32">
         <v>3.33</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+      <c r="E32" s="4">
+        <v>0.435</v>
+      </c>
+      <c r="F32" s="4">
+        <v>5.8999999999999997E-2</v>
+      </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="1">
         <v>6.66</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
+      <c r="E33" s="4">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0.11799999999999999</v>
+      </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>10</v>
       </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
+      <c r="E34" s="4">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0.11799999999999999</v>
+      </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E35">

</xml_diff>

<commit_message>
Changed how positive/negetive classes are counted in confusion func + updated xls file + saved run output to output.txt
</commit_message>
<xml_diff>
--- a/HW5/instructions/ROC First Step.xlsx
+++ b/HW5/instructions/ROC First Step.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cod\machineLearning\HW5\instructions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\arik\git\machineLearningHW\HW5\instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -55,14 +55,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -111,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -120,10 +120,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="טוב" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -146,7 +147,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="he-IL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -213,7 +214,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="he-IL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -266,22 +267,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.35899999999999999</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20499999999999999</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.23100000000000001</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10299999999999999</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0999999999999997E-2</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -293,22 +294,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.81100000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.38900000000000001</c:v>
+                  <c:v>0.83799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.44400000000000001</c:v>
+                  <c:v>0.89200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16700000000000001</c:v>
+                  <c:v>0.97299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.111</c:v>
+                  <c:v>0.97299999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -405,7 +406,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="he-IL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -443,7 +444,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="he-IL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="461477072"/>
@@ -525,7 +526,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="he-IL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -563,7 +564,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="he-IL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="461465104"/>
@@ -605,7 +606,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="he-IL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -619,7 +620,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="he-IL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -682,7 +683,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="he-IL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -762,46 +763,46 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.1999999999999999E-2</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.1999999999999999E-2</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1999999999999999E-2</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.13300000000000001</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.13300000000000001</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.17799999999999999</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -834,40 +835,40 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.94599999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0.89200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.86499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.83799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0.83799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>0.83799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>8.3000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.41699999999999998</c:v>
+                  <c:v>8.3000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.5</c:v>
+                  <c:v>0.83799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.5</c:v>
+                  <c:v>0.83799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.66700000000000004</c:v>
+                  <c:v>0.83799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.66700000000000004</c:v>
+                  <c:v>0.83799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -967,7 +968,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="he-IL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1005,7 +1006,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="he-IL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="461462928"/>
@@ -1088,7 +1089,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="he-IL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1126,7 +1127,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="he-IL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="461463472"/>
@@ -1168,7 +1169,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="he-IL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2319,8 +2320,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4876800" y="370840"/>
-          <a:ext cx="4500880" cy="4123690"/>
+          <a:off x="4495800" y="396240"/>
+          <a:ext cx="4145280" cy="4415790"/>
           <a:chOff x="5707380" y="365760"/>
           <a:chExt cx="4572000" cy="4065270"/>
         </a:xfrm>
@@ -2422,16 +2423,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>450895</xdr:colOff>
+      <xdr:colOff>508045</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>85042</xdr:rowOff>
+      <xdr:rowOff>75517</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2446,7 +2447,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5105400" y="904875"/>
+          <a:off x="5162550" y="895350"/>
           <a:ext cx="2317795" cy="2228167"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2738,16 +2739,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2759,7 +2760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -2767,13 +2768,13 @@
         <v>2</v>
       </c>
       <c r="E5" s="2">
-        <v>0.5</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="F5" s="2">
-        <v>0.35899999999999999</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>3</v>
       </c>
@@ -2781,13 +2782,13 @@
         <v>3</v>
       </c>
       <c r="E6" s="2">
-        <v>0.38900000000000001</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="F6" s="2">
-        <v>0.20499999999999999</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>3</v>
       </c>
@@ -2795,13 +2796,13 @@
         <v>4</v>
       </c>
       <c r="E7" s="2">
-        <v>0.44400000000000001</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="F7" s="2">
-        <v>0.23100000000000001</v>
+        <v>0.65</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>4</v>
       </c>
@@ -2815,7 +2816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>4</v>
       </c>
@@ -2823,13 +2824,13 @@
         <v>0.1</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16700000000000001</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="F9" s="2">
-        <v>0.10299999999999999</v>
+        <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>4</v>
       </c>
@@ -2837,13 +2838,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>0.111</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="F10" s="2">
-        <v>5.0999999999999997E-2</v>
+        <v>0.85</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>6</v>
       </c>
@@ -2857,7 +2858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
@@ -2871,7 +2872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>6.6000000000000005E-5</v>
       </c>
@@ -2882,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>1E-4</v>
       </c>
@@ -2893,7 +2894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>3.3E-4</v>
       </c>
@@ -2904,7 +2905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>6.6E-4</v>
       </c>
@@ -2912,10 +2913,10 @@
         <v>1</v>
       </c>
       <c r="F21" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>1E-3</v>
       </c>
@@ -2923,76 +2924,76 @@
         <v>1</v>
       </c>
       <c r="F22" s="4">
-        <v>1</v>
+        <v>0.85</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>3.3E-3</v>
       </c>
       <c r="E23" s="4">
-        <v>1</v>
+        <v>0.94599999999999995</v>
       </c>
       <c r="F23" s="4">
-        <v>1</v>
+        <v>0.65</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D24">
         <v>6.6E-3</v>
       </c>
       <c r="E24" s="4">
-        <v>1</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="F24" s="4">
-        <v>1</v>
+        <v>0.65</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D25">
         <v>0.01</v>
       </c>
       <c r="E25" s="4">
-        <v>1</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="F25" s="4">
-        <v>1</v>
+        <v>0.65</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="E26" s="4">
-        <v>1</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="F26" s="4">
-        <v>1</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="E27" s="4">
-        <v>1</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="F27" s="4">
-        <v>1</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>0.1</v>
       </c>
       <c r="E28" s="4">
-        <v>1</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="F28" s="4">
-        <v>1</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>0.33</v>
       </c>
@@ -3000,66 +3001,66 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="F29" s="4">
-        <v>2.1999999999999999E-2</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>0.66</v>
       </c>
       <c r="E30" s="4">
-        <v>0.41699999999999998</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="F30" s="4">
-        <v>2.1999999999999999E-2</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" s="4">
-        <v>0.5</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="F31" s="4">
-        <v>2.1999999999999999E-2</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D32">
         <v>3.33</v>
       </c>
-      <c r="E32" s="4">
-        <v>0.5</v>
+      <c r="E32" s="6">
+        <v>0.83799999999999997</v>
       </c>
       <c r="F32" s="4">
-        <v>0.13300000000000001</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="1">
         <v>6.66</v>
       </c>
       <c r="E33" s="4">
-        <v>0.66700000000000004</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="F33" s="4">
-        <v>0.13300000000000001</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>10</v>
       </c>
       <c r="E34" s="4">
-        <v>0.66700000000000004</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="F34" s="4">
-        <v>0.17799999999999999</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>0</v>
       </c>
@@ -3072,6 +3073,7 @@
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>